<commit_message>
Trigger voltage line version
</commit_message>
<xml_diff>
--- a/Data/SPIV_Setting _V02 - 複製.xlsx
+++ b/Data/SPIV_Setting _V02 - 複製.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20351"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SIV-POWER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\OneDrive - Wistron Corporation\SIV-POWER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F44EF0A-517F-4092-84B1-F803A57CFABC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA439B7-BB31-4AC7-8157-6BA356EF2060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27" yWindow="0" windowWidth="22473" windowHeight="12320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regulation" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="57">
   <si>
     <t>Imax</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1196,26 +1196,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.7"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="1"/>
-    <col min="5" max="5" width="16.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="17.21875" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.87890625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.52734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.76171875" style="1"/>
+    <col min="5" max="5" width="16.1171875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.52734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.87890625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.87890625" customWidth="1"/>
+    <col min="9" max="9" width="14.52734375" customWidth="1"/>
+    <col min="10" max="10" width="14.41015625" customWidth="1"/>
+    <col min="11" max="11" width="16.52734375" customWidth="1"/>
+    <col min="12" max="12" width="17.234375" customWidth="1"/>
+    <col min="13" max="13" width="12.3515625" customWidth="1"/>
+    <col min="14" max="14" width="11.52734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1380,17 +1380,17 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.7"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.64453125" customWidth="1"/>
+    <col min="2" max="2" width="13.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.87890625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.41015625" customWidth="1"/>
+    <col min="6" max="6" width="11.76171875" customWidth="1"/>
+    <col min="7" max="7" width="12.41015625" customWidth="1"/>
+    <col min="8" max="8" width="12.41015625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.52734375" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1514,25 +1514,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.7"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.64453125" customWidth="1"/>
+    <col min="2" max="2" width="13.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.87890625" customWidth="1"/>
+    <col min="5" max="5" width="9.1171875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.1171875" customWidth="1"/>
+    <col min="9" max="9" width="13.64453125" customWidth="1"/>
+    <col min="10" max="10" width="10.1171875" customWidth="1"/>
+    <col min="11" max="11" width="10.76171875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="24.6" customHeight="1">
@@ -1650,6 +1650,41 @@
         <v>1</v>
       </c>
       <c r="K3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5.25</v>
+      </c>
+      <c r="G4" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="H4" s="3">
+        <v>5.25</v>
+      </c>
+      <c r="I4" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1668,19 +1703,19 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.7"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.87890625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.1171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.76171875" customWidth="1"/>
+    <col min="6" max="6" width="11.52734375" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.76171875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.3515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1769,26 +1804,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C97EC8-FCEE-410B-AE35-121BC01CAE3B}">
   <dimension ref="A1:BO134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="AZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.7"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="8.88671875" style="16"/>
-    <col min="9" max="9" width="13.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="22" width="8.88671875" style="16"/>
-    <col min="24" max="38" width="8.88671875" style="16"/>
-    <col min="40" max="55" width="8.88671875" style="16"/>
-    <col min="57" max="62" width="8.88671875" style="16"/>
-    <col min="63" max="63" width="13.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.21875" style="16" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="14.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="14.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.3515625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="11.52734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="8.87890625" style="16"/>
+    <col min="9" max="9" width="13.41015625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.41015625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="22" width="8.87890625" style="16"/>
+    <col min="24" max="38" width="8.87890625" style="16"/>
+    <col min="40" max="55" width="8.87890625" style="16"/>
+    <col min="57" max="62" width="8.87890625" style="16"/>
+    <col min="63" max="63" width="13.41015625" style="16" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.234375" style="16" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="14.87890625" style="16" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="14.64453125" style="16" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="17" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2221,7 +2256,7 @@
         <v>43626</v>
       </c>
     </row>
-    <row r="8" spans="1:67" ht="31.2">
+    <row r="8" spans="1:67">
       <c r="A8" s="7" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
FIX load funtion BUG
</commit_message>
<xml_diff>
--- a/Data/SPIV_Setting _V02 - 複製.xlsx
+++ b/Data/SPIV_Setting _V02 - 複製.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\OneDrive - Wistron Corporation\SIV-POWER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA439B7-BB31-4AC7-8157-6BA356EF2060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E00401-3762-4DD6-9A80-9D3AEE71AF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27" yWindow="0" windowWidth="22473" windowHeight="12320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="907" yWindow="680" windowWidth="19200" windowHeight="10073" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regulation" sheetId="5" r:id="rId1"/>
@@ -1377,7 +1377,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.7"/>
@@ -1514,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.7"/>
@@ -1687,6 +1687,32 @@
       <c r="K4" s="3">
         <v>1</v>
       </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>